<commit_message>
Arreglos pequenos y detalles
</commit_message>
<xml_diff>
--- a/Excel/baseDatosSismos.xlsx
+++ b/Excel/baseDatosSismos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianbermudez/Documents/CodesS2/GitHub/Tarea1POO/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudianteccr-my.sharepoint.com/personal/sebastianarroniz55_estudiantec_cr/Documents/TEC/Semestre II 2021/POO/Semana 11/Proyecto I/Tarea1POO/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8D3406-65D4-B744-9803-6D6C15DDB7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4D8D3406-65D4-B744-9803-6D6C15DDB7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB3F0983-26EE-4DD3-A06C-9EA489829288}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="169">
   <si>
     <t>3.6 km Norte de Carrizal de Alajuela</t>
   </si>
@@ -523,6 +523,15 @@
   </si>
   <si>
     <t>MI casaaaaa jajaajja xd</t>
+  </si>
+  <si>
+    <t>06/10/2021</t>
+  </si>
+  <si>
+    <t>19:22:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Calle Fallas</t>
   </si>
 </sst>
 </file>
@@ -920,27 +929,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K131"/>
+  <dimension ref="A1:K132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="14" width="11.1640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="14" width="10.5" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="14" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="14" width="10.42578125" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="11" width="13.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="11" width="14.1640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="14" width="17.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="11" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="14" width="17.42578125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="4" width="20.0" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" style="17" width="12.5" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="4" width="10.1640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="14" width="20.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="6" width="11.1640625" collapsed="true"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" style="17" width="12.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="4" width="10.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="14" width="50.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="6" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>21</v>
       </c>
@@ -973,7 +982,7 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>33</v>
       </c>
@@ -1006,7 +1015,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>34</v>
       </c>
@@ -1038,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>35</v>
       </c>
@@ -1070,7 +1079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>36</v>
       </c>
@@ -1102,7 +1111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>37</v>
       </c>
@@ -1134,7 +1143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
@@ -1166,7 +1175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>39</v>
       </c>
@@ -1198,7 +1207,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>40</v>
       </c>
@@ -1230,7 +1239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>41</v>
       </c>
@@ -1262,7 +1271,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>42</v>
       </c>
@@ -1294,7 +1303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>43</v>
       </c>
@@ -1326,7 +1335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>44</v>
       </c>
@@ -1358,7 +1367,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>45</v>
       </c>
@@ -1390,7 +1399,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>46</v>
       </c>
@@ -1422,7 +1431,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>47</v>
       </c>
@@ -1454,7 +1463,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>48</v>
       </c>
@@ -1486,7 +1495,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>49</v>
       </c>
@@ -1518,7 +1527,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>50</v>
       </c>
@@ -1550,7 +1559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>51</v>
       </c>
@@ -1583,7 +1592,7 @@
       </c>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>52</v>
       </c>
@@ -1615,7 +1624,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -1648,7 +1657,7 @@
       </c>
       <c r="K22"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -1681,7 +1690,7 @@
       </c>
       <c r="K23"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -1714,7 +1723,7 @@
       </c>
       <c r="K24"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -1747,7 +1756,7 @@
       </c>
       <c r="K25"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -1780,7 +1789,7 @@
       </c>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -1813,7 +1822,7 @@
       </c>
       <c r="K27"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -1846,7 +1855,7 @@
       </c>
       <c r="K28"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>96</v>
       </c>
@@ -1879,7 +1888,7 @@
       </c>
       <c r="K29"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -1912,7 +1921,7 @@
       </c>
       <c r="K30"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>99</v>
       </c>
@@ -1945,7 +1954,7 @@
       </c>
       <c r="K31"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>99</v>
       </c>
@@ -1978,7 +1987,7 @@
       </c>
       <c r="K32"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -2011,7 +2020,7 @@
       </c>
       <c r="K33"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>99</v>
       </c>
@@ -2044,7 +2053,7 @@
       </c>
       <c r="K34"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -2077,7 +2086,7 @@
       </c>
       <c r="K35"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>99</v>
       </c>
@@ -2109,7 +2118,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -2141,7 +2150,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -2173,7 +2182,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>115</v>
       </c>
@@ -2205,7 +2214,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -2237,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -2269,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -2301,7 +2310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2333,7 +2342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -2365,7 +2374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -2397,7 +2406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -2429,7 +2438,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -2461,7 +2470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -2493,7 +2502,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -2525,7 +2534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -2557,7 +2566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -2589,7 +2598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>45</v>
       </c>
@@ -2621,7 +2630,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -2653,7 +2662,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -2685,7 +2694,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -2717,7 +2726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -2749,7 +2758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -2781,7 +2790,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -2813,7 +2822,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>52</v>
       </c>
@@ -2845,7 +2854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>73</v>
       </c>
@@ -2877,7 +2886,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -2909,7 +2918,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -2941,7 +2950,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -2973,7 +2982,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>87</v>
       </c>
@@ -3005,7 +3014,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>90</v>
       </c>
@@ -3037,7 +3046,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>93</v>
       </c>
@@ -3069,7 +3078,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>96</v>
       </c>
@@ -3101,7 +3110,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>99</v>
       </c>
@@ -3133,7 +3142,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>99</v>
       </c>
@@ -3165,7 +3174,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>101</v>
       </c>
@@ -3197,7 +3206,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>99</v>
       </c>
@@ -3229,7 +3238,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>105</v>
       </c>
@@ -3261,7 +3270,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>99</v>
       </c>
@@ -3293,7 +3302,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>99</v>
       </c>
@@ -3325,7 +3334,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>99</v>
       </c>
@@ -3357,7 +3366,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>115</v>
       </c>
@@ -3389,7 +3398,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>33</v>
       </c>
@@ -3421,7 +3430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>34</v>
       </c>
@@ -3453,7 +3462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>35</v>
       </c>
@@ -3485,7 +3494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>36</v>
       </c>
@@ -3517,7 +3526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>37</v>
       </c>
@@ -3549,7 +3558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>38</v>
       </c>
@@ -3581,7 +3590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>39</v>
       </c>
@@ -3613,7 +3622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>40</v>
       </c>
@@ -3645,7 +3654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>41</v>
       </c>
@@ -3677,7 +3686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>42</v>
       </c>
@@ -3709,7 +3718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>43</v>
       </c>
@@ -3741,7 +3750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>44</v>
       </c>
@@ -3773,7 +3782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>45</v>
       </c>
@@ -3805,7 +3814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>46</v>
       </c>
@@ -3837,7 +3846,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>47</v>
       </c>
@@ -3869,7 +3878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -3901,7 +3910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>49</v>
       </c>
@@ -3933,7 +3942,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>50</v>
       </c>
@@ -3965,7 +3974,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>51</v>
       </c>
@@ -3997,7 +4006,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>52</v>
       </c>
@@ -4029,7 +4038,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>73</v>
       </c>
@@ -4061,7 +4070,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>76</v>
       </c>
@@ -4093,7 +4102,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>80</v>
       </c>
@@ -4125,7 +4134,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>84</v>
       </c>
@@ -4157,7 +4166,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>87</v>
       </c>
@@ -4189,7 +4198,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>90</v>
       </c>
@@ -4221,7 +4230,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>93</v>
       </c>
@@ -4253,7 +4262,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>96</v>
       </c>
@@ -4285,7 +4294,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>99</v>
       </c>
@@ -4317,7 +4326,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>99</v>
       </c>
@@ -4349,7 +4358,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>101</v>
       </c>
@@ -4381,7 +4390,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>99</v>
       </c>
@@ -4413,7 +4422,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>105</v>
       </c>
@@ -4445,7 +4454,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>99</v>
       </c>
@@ -4477,7 +4486,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>99</v>
       </c>
@@ -4509,7 +4518,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>99</v>
       </c>
@@ -4541,7 +4550,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>115</v>
       </c>
@@ -4573,7 +4582,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>115</v>
       </c>
@@ -4605,7 +4614,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>115</v>
       </c>
@@ -4637,7 +4646,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>124</v>
       </c>
@@ -4669,7 +4678,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>127</v>
       </c>
@@ -4701,7 +4710,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>129</v>
       </c>
@@ -4733,7 +4742,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>115</v>
       </c>
@@ -4765,7 +4774,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>115</v>
       </c>
@@ -4797,7 +4806,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>135</v>
       </c>
@@ -4829,7 +4838,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>138</v>
       </c>
@@ -4861,7 +4870,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>115</v>
       </c>
@@ -4893,7 +4902,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>115</v>
       </c>
@@ -4925,7 +4934,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>145</v>
       </c>
@@ -4957,196 +4966,228 @@
         <v>147</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>149</v>
       </c>
       <c r="B126" t="s">
         <v>150</v>
       </c>
-      <c r="C126" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="D126" t="n">
-        <v>7.0</v>
+      <c r="C126">
+        <v>36</v>
+      </c>
+      <c r="D126">
+        <v>7</v>
       </c>
       <c r="E126" t="s">
         <v>78</v>
       </c>
-      <c r="F126" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="G126" t="n">
-        <v>-29832.0</v>
-      </c>
-      <c r="H126" t="n">
-        <v>-23.0</v>
-      </c>
-      <c r="I126" t="n">
-        <v>2.0</v>
+      <c r="F126">
+        <v>6</v>
+      </c>
+      <c r="G126">
+        <v>-29832</v>
+      </c>
+      <c r="H126">
+        <v>-23</v>
+      </c>
+      <c r="I126">
+        <v>2</v>
       </c>
       <c r="J126" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>152</v>
       </c>
       <c r="B127" t="s">
         <v>153</v>
       </c>
-      <c r="C127" t="n">
-        <v>33.3</v>
-      </c>
-      <c r="D127" t="n">
+      <c r="C127">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="D127">
         <v>3.4</v>
       </c>
       <c r="E127" t="s">
         <v>30</v>
       </c>
-      <c r="F127" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="G127" t="n">
-        <v>-324.4</v>
-      </c>
-      <c r="H127" t="n">
+      <c r="F127">
+        <v>7</v>
+      </c>
+      <c r="G127">
+        <v>-324.39999999999998</v>
+      </c>
+      <c r="H127">
         <v>23.69</v>
       </c>
-      <c r="I127" t="n">
-        <v>2.0</v>
+      <c r="I127">
+        <v>2</v>
       </c>
       <c r="J127" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>155</v>
       </c>
       <c r="B128" t="s">
         <v>156</v>
       </c>
-      <c r="C128" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="D128" t="n">
-        <v>23.0</v>
+      <c r="C128">
+        <v>45</v>
+      </c>
+      <c r="D128">
+        <v>23</v>
       </c>
       <c r="E128" t="s">
         <v>78</v>
       </c>
-      <c r="F128" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G128" t="n">
+      <c r="F128">
+        <v>1</v>
+      </c>
+      <c r="G128">
         <v>-23.5</v>
       </c>
-      <c r="H128" t="n">
+      <c r="H128">
         <v>232.23</v>
       </c>
-      <c r="I128" t="n">
-        <v>1.0</v>
+      <c r="I128">
+        <v>1</v>
       </c>
       <c r="J128" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>158</v>
       </c>
       <c r="B129" t="s">
         <v>159</v>
       </c>
-      <c r="C129" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="D129" t="n">
-        <v>4.0</v>
+      <c r="C129">
+        <v>45</v>
+      </c>
+      <c r="D129">
+        <v>4</v>
       </c>
       <c r="E129" t="s">
         <v>30</v>
       </c>
-      <c r="F129" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G129" t="n">
-        <v>-400.0</v>
-      </c>
-      <c r="H129" t="n">
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="G129">
+        <v>-400</v>
+      </c>
+      <c r="H129">
         <v>809.1</v>
       </c>
-      <c r="I129" t="n">
-        <v>1.0</v>
+      <c r="I129">
+        <v>1</v>
       </c>
       <c r="J129" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>158</v>
       </c>
       <c r="B130" t="s">
         <v>161</v>
       </c>
-      <c r="C130" t="n">
-        <v>23.0</v>
-      </c>
-      <c r="D130" t="n">
-        <v>2.0</v>
+      <c r="C130">
+        <v>23</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
       </c>
       <c r="E130" t="s">
         <v>82</v>
       </c>
-      <c r="F130" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="G130" t="n">
+      <c r="F130">
+        <v>3</v>
+      </c>
+      <c r="G130">
         <v>200.62</v>
       </c>
-      <c r="H130" t="n">
+      <c r="H130">
         <v>100.59</v>
       </c>
-      <c r="I130" t="n">
-        <v>2.0</v>
+      <c r="I130">
+        <v>2</v>
       </c>
       <c r="J130" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>163</v>
       </c>
       <c r="B131" t="s">
         <v>164</v>
       </c>
-      <c r="C131" t="n">
-        <v>1222.0</v>
-      </c>
-      <c r="D131" t="n">
-        <v>23.0</v>
+      <c r="C131">
+        <v>1222</v>
+      </c>
+      <c r="D131">
+        <v>23</v>
       </c>
       <c r="E131" t="s">
         <v>30</v>
       </c>
-      <c r="F131" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="G131" t="n">
-        <v>-123.0</v>
-      </c>
-      <c r="H131" t="n">
-        <v>222.0</v>
-      </c>
-      <c r="I131" t="n">
-        <v>2.0</v>
+      <c r="F131">
+        <v>7</v>
+      </c>
+      <c r="G131">
+        <v>-123</v>
+      </c>
+      <c r="H131">
+        <v>222</v>
+      </c>
+      <c r="I131">
+        <v>2</v>
       </c>
       <c r="J131" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>166</v>
+      </c>
+      <c r="B132" t="s">
+        <v>167</v>
+      </c>
+      <c r="C132" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="D132" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="E132" t="s">
+        <v>29</v>
+      </c>
+      <c r="F132" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G132" t="n">
+        <v>3087.43</v>
+      </c>
+      <c r="H132" t="n">
+        <v>-88092.902</v>
+      </c>
+      <c r="I132" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J132" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -5386,18 +5427,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5420,14 +5461,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4292BCCE-7308-4F70-A272-6B4ADAEE3B4B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84BF098F-A7EB-4925-BB55-245E4CAE68F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5442,4 +5475,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4292BCCE-7308-4F70-A272-6B4ADAEE3B4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>